<commit_message>
[ADD] Gouges to brake app
</commit_message>
<xml_diff>
--- a/parameters/UFSC.xlsx
+++ b/parameters/UFSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\TIA\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE821861-A3E5-4010-9A59-D1CE2BF051D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF8D30C-978F-43C1-8739-40D112C24790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="2970" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -99,13 +99,13 @@
     <t>3.91</t>
   </si>
   <si>
-    <t>3.07</t>
-  </si>
-  <si>
     <t>15.83</t>
   </si>
   <si>
     <t>7.16</t>
+  </si>
+  <si>
+    <t>3.08</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
@@ -271,9 +271,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -562,7 +559,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +615,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -635,10 +632,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -699,7 +696,6 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="14"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>